<commit_message>
before major change in shark tic report
</commit_message>
<xml_diff>
--- a/voldailyanalytics/result.xlsx
+++ b/voldailyanalytics/result.xlsx
@@ -529,13 +529,13 @@
         <v>-30</v>
       </c>
       <c r="E2">
-        <v>0.19</v>
+        <v>0.16</v>
       </c>
       <c r="F2">
-        <v>0.2</v>
+        <v>0.17</v>
       </c>
       <c r="G2">
-        <v>0.19</v>
+        <v>0.16</v>
       </c>
       <c r="H2">
         <v>-560.4</v>
@@ -547,34 +547,34 @@
         <v>100</v>
       </c>
       <c r="K2">
-        <v>0.0729326494543058</v>
+        <v>0.0635327980336118</v>
       </c>
       <c r="L2">
-        <v>0.0234332464367131</v>
+        <v>0.0210419003076321</v>
       </c>
       <c r="M2">
-        <v>-0.0134703649950669</v>
+        <v>-0.0117312964988799</v>
       </c>
       <c r="N2">
-        <v>0.0998795493702728</v>
+        <v>0.0816093863996498</v>
       </c>
       <c r="O2" s="2">
-        <v>42633.6611689815</v>
+        <v>42632.9111111111</v>
       </c>
       <c r="P2" s="2">
         <v>42633.6541666667</v>
       </c>
       <c r="Q2">
-        <v>0.0948928718800891</v>
+        <v>0.0936522598789154</v>
       </c>
       <c r="R2" s="2">
         <v>42664</v>
       </c>
       <c r="S2">
-        <v>214.04</v>
+        <v>213.6</v>
       </c>
       <c r="T2">
-        <v>-585</v>
+        <v>-495</v>
       </c>
     </row>
     <row r="3" spans="1:20">
@@ -596,6 +596,9 @@
       <c r="F3">
         <v>0.04</v>
       </c>
+      <c r="G3">
+        <v>0.03</v>
+      </c>
       <c r="H3">
         <v>90.47</v>
       </c>
@@ -606,31 +609,31 @@
         <v>100</v>
       </c>
       <c r="K3">
-        <v>0.0083284821006327</v>
+        <v>0.00729229547981208</v>
       </c>
       <c r="L3">
-        <v>0.00401679390093535</v>
+        <v>0.00353121961828463</v>
       </c>
       <c r="M3">
-        <v>-0.00205783550575824</v>
+        <v>-0.00180588978926703</v>
       </c>
       <c r="N3">
-        <v>0.0199182977436275</v>
+        <v>0.0176913090918269</v>
       </c>
       <c r="O3" s="2">
-        <v>42633.6611689815</v>
+        <v>42632.9111111111</v>
       </c>
       <c r="P3" s="2">
         <v>42633.6541666667</v>
       </c>
       <c r="Q3">
-        <v>0.0897754934672465</v>
+        <v>0.089888083175986</v>
       </c>
       <c r="R3" s="2">
         <v>42664</v>
       </c>
       <c r="S3">
-        <v>214.04</v>
+        <v>213.6</v>
       </c>
       <c r="T3">
         <v>105</v>
@@ -650,13 +653,13 @@
         <v>30</v>
       </c>
       <c r="E4">
-        <v>0.4</v>
+        <v>0.44</v>
       </c>
       <c r="F4">
-        <v>0.41</v>
+        <v>0.45</v>
       </c>
       <c r="G4">
-        <v>0.4</v>
+        <v>0.47</v>
       </c>
       <c r="H4">
         <v>1199.81</v>
@@ -668,34 +671,34 @@
         <v>100</v>
       </c>
       <c r="K4">
-        <v>-0.0646400587875333</v>
+        <v>-0.0695550996747478</v>
       </c>
       <c r="L4">
-        <v>0.00936571037406362</v>
+        <v>0.00989485314167953</v>
       </c>
       <c r="M4">
-        <v>-0.0273595916462556</v>
+        <v>-0.0285708991382583</v>
       </c>
       <c r="N4">
-        <v>0.075514934147724</v>
+        <v>0.100302169534225</v>
       </c>
       <c r="O4" s="2">
-        <v>42633.6611689815</v>
+        <v>42632.9111111111</v>
       </c>
       <c r="P4" s="2">
         <v>42633.6541666667</v>
       </c>
       <c r="Q4">
-        <v>0.216572973464648</v>
+        <v>0.215777176360249</v>
       </c>
       <c r="R4" s="2">
         <v>42664</v>
       </c>
       <c r="S4">
-        <v>214.04</v>
+        <v>213.6</v>
       </c>
       <c r="T4">
-        <v>1215</v>
+        <v>1335</v>
       </c>
     </row>
     <row r="5" spans="1:20">
@@ -712,13 +715,13 @@
         <v>-30</v>
       </c>
       <c r="E5">
-        <v>0.67</v>
+        <v>0.74</v>
       </c>
       <c r="F5">
-        <v>0.68</v>
+        <v>0.75</v>
       </c>
       <c r="G5">
-        <v>0.66</v>
+        <v>0.74</v>
       </c>
       <c r="H5">
         <v>-2009.71</v>
@@ -730,34 +733,34 @@
         <v>100</v>
       </c>
       <c r="K5">
-        <v>-0.106869411433907</v>
+        <v>-0.115897941048817</v>
       </c>
       <c r="L5">
-        <v>0.0152594996994505</v>
+        <v>0.0161839028817106</v>
       </c>
       <c r="M5">
-        <v>-0.035649461506943</v>
+        <v>-0.0372310404313283</v>
       </c>
       <c r="N5">
-        <v>0.106553845334</v>
+        <v>0.135854956008718</v>
       </c>
       <c r="O5" s="2">
-        <v>42633.6611689815</v>
+        <v>42632.9111111111</v>
       </c>
       <c r="P5" s="2">
         <v>42633.6541666667</v>
       </c>
       <c r="Q5">
-        <v>0.193794118459042</v>
+        <v>0.192828773389221</v>
       </c>
       <c r="R5" s="2">
         <v>42664</v>
       </c>
       <c r="S5">
-        <v>214.13</v>
+        <v>213.58</v>
       </c>
       <c r="T5">
-        <v>-2025</v>
+        <v>-2235</v>
       </c>
     </row>
   </sheetData>

</xml_diff>